<commit_message>
Commit for setup change
</commit_message>
<xml_diff>
--- a/FacebookAutomation/src/test/resources/Credentials.xlsx
+++ b/FacebookAutomation/src/test/resources/Credentials.xlsx
@@ -5,17 +5,16 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FacebookAutomation\FacebookAutomation\FacebookAutomation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FacebookAutomation\FacebookAutomation\FacebookAutomation\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16884" windowHeight="3108"/>
   </bookViews>
   <sheets>
-    <sheet name="Setupdetails" sheetId="1" r:id="rId1"/>
-    <sheet name="LoginDetails" sheetId="2" r:id="rId2"/>
+    <sheet name="testCaseData" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,39 +24,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
-  <si>
-    <t>WebApplication Automation</t>
-  </si>
-  <si>
-    <t>URL &amp; Browser details</t>
-  </si>
-  <si>
-    <t>URL</t>
-  </si>
-  <si>
-    <t>Browser</t>
-  </si>
-  <si>
-    <t>Firefox</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/</t>
-  </si>
-  <si>
-    <t>Credentials</t>
-  </si>
-  <si>
-    <t>email</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>nivipriya1001@gmail.com</t>
+  </si>
+  <si>
+    <t>Lotica@123</t>
+  </si>
+  <si>
+    <t>TestCaseID</t>
+  </si>
+  <si>
+    <t>emailID</t>
   </si>
   <si>
     <t>password</t>
   </si>
   <si>
-    <t>nivipriya1001@gmail.com</t>
-  </si>
-  <si>
-    <t>Lotica@123</t>
+    <t>TC001_invalidemail</t>
+  </si>
+  <si>
+    <t>TC002_invalidpassword</t>
+  </si>
+  <si>
+    <t>TC003_validlogin</t>
+  </si>
+  <si>
+    <t>test123@yahoo.com</t>
+  </si>
+  <si>
+    <t>test@123</t>
+  </si>
+  <si>
+    <t>abc@gmail.com</t>
+  </si>
+  <si>
+    <t>Test@123</t>
   </si>
 </sst>
 </file>
@@ -73,14 +75,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
@@ -88,8 +82,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -98,18 +100,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="1" tint="4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -132,105 +128,17 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -512,116 +420,73 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" customWidth="1"/>
-    <col min="2" max="2" width="24.5546875" customWidth="1"/>
+    <col min="1" max="1" width="35" customWidth="1"/>
+    <col min="2" max="2" width="45.88671875" customWidth="1"/>
     <col min="3" max="3" width="53.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="6"/>
+        <v>2</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="8"/>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:A3"/>
-  </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3">
-      <formula1>"Chrome,Firefox,Edge"</formula1>
-    </dataValidation>
-  </dataValidations>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId2"/>
+    <hyperlink ref="B3" r:id="rId3"/>
+    <hyperlink ref="C3" r:id="rId4"/>
+    <hyperlink ref="B4" r:id="rId5"/>
+    <hyperlink ref="C4" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="17.88671875" customWidth="1"/>
-    <col min="2" max="2" width="29.21875" customWidth="1"/>
-    <col min="3" max="3" width="43.77734375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="11"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="8"/>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:A3"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Commit for entire setup and testmodule change
</commit_message>
<xml_diff>
--- a/FacebookAutomation/src/test/resources/Credentials.xlsx
+++ b/FacebookAutomation/src/test/resources/Credentials.xlsx
@@ -3,6 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FacebookAutomation\FacebookAutomation\FacebookAutomation\src\test\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16884" windowHeight="3108"/>
   </bookViews>
@@ -10,7 +15,6 @@
     <sheet name="testCaseData" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -46,9 +50,6 @@
     <t>TC003_validlogin</t>
   </si>
   <si>
-    <t>test123@yahoo.com</t>
-  </si>
-  <si>
     <t>test@123</t>
   </si>
   <si>
@@ -56,6 +57,9 @@
   </si>
   <si>
     <t>Test@123</t>
+  </si>
+  <si>
+    <t>gowtham@yahoo.com</t>
   </si>
 </sst>
 </file>
@@ -419,7 +423,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B16" activeCellId="1" sqref="B2 B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -445,10 +449,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -456,10 +460,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
commit for loginPage module
</commit_message>
<xml_diff>
--- a/FacebookAutomation/src/test/resources/Credentials.xlsx
+++ b/FacebookAutomation/src/test/resources/Credentials.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Lotica@123</t>
   </si>
@@ -38,15 +38,6 @@
     <t>password</t>
   </si>
   <si>
-    <t>TC001_invalidemail</t>
-  </si>
-  <si>
-    <t>TC002_invalidpassword</t>
-  </si>
-  <si>
-    <t>TC003_validlogin</t>
-  </si>
-  <si>
     <t>test@123</t>
   </si>
   <si>
@@ -60,6 +51,18 @@
   </si>
   <si>
     <t>lotica.aitech@gmail.com</t>
+  </si>
+  <si>
+    <t>TC001_LoginPageValidation</t>
+  </si>
+  <si>
+    <t>TC002_invalidemail</t>
+  </si>
+  <si>
+    <t>TC003_invalidpassword</t>
+  </si>
+  <si>
+    <t>TC004_validlogin</t>
   </si>
 </sst>
 </file>
@@ -420,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -446,45 +449,52 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>7</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="2" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="C2" r:id="rId2"/>
-    <hyperlink ref="B3" r:id="rId3"/>
-    <hyperlink ref="C3" r:id="rId4"/>
-    <hyperlink ref="B4" r:id="rId5"/>
-    <hyperlink ref="C4" r:id="rId6"/>
+    <hyperlink ref="B4" r:id="rId1"/>
+    <hyperlink ref="C4" r:id="rId2"/>
+    <hyperlink ref="B5" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="B3" r:id="rId5"/>
+    <hyperlink ref="C3" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>

</xml_diff>

<commit_message>
commit for ui testcase
</commit_message>
<xml_diff>
--- a/FacebookAutomation/src/test/resources/Credentials.xlsx
+++ b/FacebookAutomation/src/test/resources/Credentials.xlsx
@@ -53,16 +53,16 @@
     <t>lotica.aitech@gmail.com</t>
   </si>
   <si>
-    <t>TC001_LoginPageValidation</t>
-  </si>
-  <si>
-    <t>TC002_invalidemail</t>
-  </si>
-  <si>
-    <t>TC003_invalidpassword</t>
-  </si>
-  <si>
-    <t>TC004_validlogin</t>
+    <t>TC001_loginPageValidation</t>
+  </si>
+  <si>
+    <t>TC002_invalidEmail</t>
+  </si>
+  <si>
+    <t>TC003_invalidPassword</t>
+  </si>
+  <si>
+    <t>TC004_validLogin</t>
   </si>
 </sst>
 </file>
@@ -426,7 +426,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>